<commit_message>
Running Tests for report
</commit_message>
<xml_diff>
--- a/Mikroprojekt2/Czas.xlsx
+++ b/Mikroprojekt2/Czas.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Macie\OneDrive\Dokumenty\GitHub\git\PiAA\Mikroprojekt2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8869EEF-95F1-433C-9387-A7023583F78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,151 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+  <si>
+    <t>Liczba elementów</t>
+  </si>
+  <si>
+    <t>Quicksort</t>
+  </si>
+  <si>
+    <t>Bucketsort</t>
+  </si>
+  <si>
+    <t>LoadData</t>
+  </si>
+  <si>
+    <t>199.948</t>
+  </si>
+  <si>
+    <t>13.013</t>
+  </si>
+  <si>
+    <t>33.547</t>
+  </si>
+  <si>
+    <t>22.023</t>
+  </si>
+  <si>
+    <t>418.75</t>
+  </si>
+  <si>
+    <t>26.532</t>
+  </si>
+  <si>
+    <t>68.568</t>
+  </si>
+  <si>
+    <t>49.056</t>
+  </si>
+  <si>
+    <t>607.671</t>
+  </si>
+  <si>
+    <t>40.038</t>
+  </si>
+  <si>
+    <t>100.835</t>
+  </si>
+  <si>
+    <t>75.515</t>
+  </si>
+  <si>
+    <t>807.939</t>
+  </si>
+  <si>
+    <t>54.834</t>
+  </si>
+  <si>
+    <t>136.176</t>
+  </si>
+  <si>
+    <t>105.076</t>
+  </si>
+  <si>
+    <t>1007.43</t>
+  </si>
+  <si>
+    <t>72.37</t>
+  </si>
+  <si>
+    <t>159.749</t>
+  </si>
+  <si>
+    <t>129.171</t>
+  </si>
+  <si>
+    <t>1211.8</t>
+  </si>
+  <si>
+    <t>87.278</t>
+  </si>
+  <si>
+    <t>190.906</t>
+  </si>
+  <si>
+    <t>167.258</t>
+  </si>
+  <si>
+    <t>1410.02</t>
+  </si>
+  <si>
+    <t>108.666</t>
+  </si>
+  <si>
+    <t>227.134</t>
+  </si>
+  <si>
+    <t>197.721</t>
+  </si>
+  <si>
+    <t>1579.71</t>
+  </si>
+  <si>
+    <t>114.419</t>
+  </si>
+  <si>
+    <t>266.448</t>
+  </si>
+  <si>
+    <t>220.061</t>
+  </si>
+  <si>
+    <t>1822.54</t>
+  </si>
+  <si>
+    <t>139.143</t>
+  </si>
+  <si>
+    <t>296.636</t>
+  </si>
+  <si>
+    <t>255.486</t>
+  </si>
+  <si>
+    <t>1936.39</t>
+  </si>
+  <si>
+    <t>143.712</t>
+  </si>
+  <si>
+    <t>309.383</t>
+  </si>
+  <si>
+    <t>276.128</t>
+  </si>
+  <si>
+    <t>[ms]</t>
+  </si>
+  <si>
+    <t>Mergesort</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -37,7 +186,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,15 +194,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +495,223 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="D3:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D5" s="1">
+        <v>100000</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D6" s="1">
+        <v>200000</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D7" s="1">
+        <v>300000</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D8" s="1">
+        <v>400000</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D9" s="1">
+        <v>500000</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D10" s="1">
+        <v>600000</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D11" s="1">
+        <v>700000</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D12" s="1">
+        <v>800000</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D13" s="1">
+        <v>900000</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D14" s="1">
+        <v>962903</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>